<commit_message>
Adjusting V_reg resistors to use 10k var res
</commit_message>
<xml_diff>
--- a/Power Supply/Power_Block/Power_Block_BOM.xlsx
+++ b/Power Supply/Power_Block/Power_Block_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Part Number</t>
   </si>
@@ -34,6 +34,24 @@
     <t>Manufacturer</t>
   </si>
   <si>
+    <t>CRCW0603910RFKEA</t>
+  </si>
+  <si>
+    <t>RES, SMD 910 OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>910 Ohm</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
     <t>RC0603JR-070RL</t>
   </si>
   <si>
@@ -43,22 +61,52 @@
     <t>0 Ohm</t>
   </si>
   <si>
-    <t>R0603</t>
-  </si>
-  <si>
     <t>R3, R4</t>
   </si>
   <si>
     <t>YAGEO</t>
   </si>
   <si>
+    <t>CRCW08054K70FKEAC</t>
+  </si>
+  <si>
+    <t>RES, 4.7K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>4.7 kOhms</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>ESK228M025AL4AA</t>
+  </si>
+  <si>
+    <t>CAP, ALUM 2200UF 20% 25V RADIAL</t>
+  </si>
+  <si>
+    <t>2200uF</t>
+  </si>
+  <si>
+    <t>ESK228M</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
     <t>FG18X7R1E105KRT00</t>
   </si>
   <si>
     <t>CAP, CER 1UF 25V X7R RADIAL</t>
   </si>
   <si>
-    <t>1u</t>
+    <t>1uF</t>
   </si>
   <si>
     <t>C-EU025-024X044</t>
@@ -76,40 +124,10 @@
     <t>CAP CER 2.2UF 10V X7R RADIAL</t>
   </si>
   <si>
-    <t>2.2u</t>
+    <t>2.2uF</t>
   </si>
   <si>
     <t>C5, C7</t>
-  </si>
-  <si>
-    <t>RC0603JR-07180RL</t>
-  </si>
-  <si>
-    <t>RES, 180 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>180 Ohm</t>
-  </si>
-  <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
-    <t>ESK228M025AL4AA</t>
-  </si>
-  <si>
-    <t>CAP, ALUM 2200UF 20% 25V RADIAL</t>
-  </si>
-  <si>
-    <t>2200uF</t>
-  </si>
-  <si>
-    <t>ESK228M</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
-    <t>KEMET</t>
   </si>
   <si>
     <t>CONN, HEADER VERT 2POS 2.54MM</t>
@@ -501,9 +519,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="25.25"/>
-    <col customWidth="1" min="3" max="3" width="29.88"/>
+    <col customWidth="1" min="3" max="3" width="35.5"/>
     <col customWidth="1" min="6" max="7" width="19.38"/>
-    <col customWidth="1" min="8" max="8" width="15.13"/>
+    <col customWidth="1" min="8" max="8" width="18.38"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -556,142 +574,144 @@
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>2.0</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="2">
         <v>2.0</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2">
         <v>2.0</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="3">
+      <c r="G8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3">
         <v>2.2232021E7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>1.0</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2">
         <v>1.0</v>
@@ -701,134 +721,155 @@
         <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2">
         <v>1.0</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2">
         <v>1.0</v>
       </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2">
         <v>1.0</v>
       </c>
-      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2">
         <v>1.0</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2">
         <v>1.0</v>
       </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>1.0</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated fuse holder F1 and a BOM
</commit_message>
<xml_diff>
--- a/Power Supply/Power_Block/Power_Block_BOM.xlsx
+++ b/Power Supply/Power_Block/Power_Block_BOM.xlsx
@@ -154,10 +154,10 @@
     <t>JST Sales America Inc.</t>
   </si>
   <si>
-    <t>F6094-ND</t>
-  </si>
-  <si>
-    <t>FUSE BLOCK CARTRIDGE PCB</t>
+    <t>3-132-873</t>
+  </si>
+  <si>
+    <t>OGN FUSEHOLDER 5X20, 22.5 MM PITCH</t>
   </si>
   <si>
     <t>5mm x 20mm</t>
@@ -166,7 +166,7 @@
     <t>F1</t>
   </si>
   <si>
-    <t>Littelfuse Inc.</t>
+    <t>SCHURTER Inc.</t>
   </si>
   <si>
     <t>L7812ACV</t>

</xml_diff>